<commit_message>
[Update] res.xlsx last version
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -1065,52 +1065,52 @@
         <v>33</v>
       </c>
       <c r="B11" t="n">
-        <v>2.559290031779848</v>
+        <v>2.523952683481694</v>
       </c>
       <c r="C11" t="n">
-        <v>2.273365870591065</v>
+        <v>2.245557781762061</v>
       </c>
       <c r="D11" t="n">
-        <v>1.985841682762736</v>
+        <v>1.965292524346421</v>
       </c>
       <c r="E11" t="n">
-        <v>1.81505685608932</v>
+        <v>1.798699734995178</v>
       </c>
       <c r="F11" t="n">
-        <v>1.691842143870376</v>
+        <v>1.678489209171317</v>
       </c>
       <c r="G11" t="n">
-        <v>1.514416251074016</v>
+        <v>1.50549253076452</v>
       </c>
       <c r="H11" t="n">
-        <v>1.29211120946589</v>
+        <v>1.29005654150989</v>
       </c>
       <c r="I11" t="n">
-        <v>1.224527644849392</v>
+        <v>1.228425208407695</v>
       </c>
       <c r="J11" t="n">
-        <v>1.292631552459659</v>
+        <v>1.296715213156989</v>
       </c>
       <c r="K11" t="n">
-        <v>1.363221242308356</v>
+        <v>1.366467934507143</v>
       </c>
       <c r="L11" t="n">
-        <v>1.472940073486299</v>
+        <v>1.474669289784171</v>
       </c>
       <c r="M11" t="n">
-        <v>1.669818850056203</v>
+        <v>1.668651422839158</v>
       </c>
       <c r="N11" t="n">
-        <v>1.871268382473745</v>
+        <v>1.866958557192161</v>
       </c>
       <c r="O11" t="s">
         <v>33</v>
       </c>
       <c r="P11" t="n">
-        <v>12.60711555476418</v>
+        <v>12.43528614073925</v>
       </c>
       <c r="Q11" t="n">
-        <v>109.5821680202657</v>
+        <v>109.1068896340253</v>
       </c>
       <c r="R11" t="s"/>
       <c r="S11" t="s">
@@ -1150,52 +1150,52 @@
         <v>34</v>
       </c>
       <c r="B12" t="n">
-        <v>7.096066610754388</v>
+        <v>8.636587370982896</v>
       </c>
       <c r="C12" t="n">
-        <v>21.00209546272253</v>
+        <v>24.51602330310273</v>
       </c>
       <c r="D12" t="n">
-        <v>69.07646324077359</v>
+        <v>82.10444858633001</v>
       </c>
       <c r="E12" t="n">
-        <v>153.9571888993609</v>
+        <v>182.3540481148718</v>
       </c>
       <c r="F12" t="n">
-        <v>299.8239850708557</v>
+        <v>337.667636511364</v>
       </c>
       <c r="G12" t="n">
-        <v>894.5404803415428</v>
+        <v>937.7923046339511</v>
       </c>
       <c r="H12" t="n">
-        <v>4713.905649465486</v>
+        <v>4783.045713271225</v>
       </c>
       <c r="I12" t="n">
-        <v>20466.73871282141</v>
+        <v>20657.72492187663</v>
       </c>
       <c r="J12" t="n">
-        <v>41807.85165349356</v>
+        <v>41559.42746431254</v>
       </c>
       <c r="K12" t="n">
-        <v>63138.24966786694</v>
+        <v>61482.02086622499</v>
       </c>
       <c r="L12" t="n">
-        <v>101487.5058237617</v>
+        <v>99227.79640890517</v>
       </c>
       <c r="M12" t="n">
-        <v>206437.9419586897</v>
+        <v>194008.5614032715</v>
       </c>
       <c r="N12" t="n">
-        <v>380706.8698266411</v>
+        <v>354829.3493756181</v>
       </c>
       <c r="O12" t="s">
         <v>34</v>
       </c>
       <c r="P12" t="n">
-        <v>851.9939223402017</v>
+        <v>763.3388887773664</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.01217548326629231</v>
+        <v>0.01150516414986073</v>
       </c>
       <c r="R12" t="s"/>
       <c r="S12" t="s">
@@ -1235,52 +1235,52 @@
         <v>37</v>
       </c>
       <c r="B13" t="n">
-        <v>10.10402113749864</v>
+        <v>12.03155630896678</v>
       </c>
       <c r="C13" t="n">
-        <v>27.69607062007132</v>
+        <v>31.38551582130729</v>
       </c>
       <c r="D13" t="n">
-        <v>87.50146067213601</v>
+        <v>98.2360995451056</v>
       </c>
       <c r="E13" t="n">
-        <v>188.037498558242</v>
+        <v>210.7505610033742</v>
       </c>
       <c r="F13" t="n">
-        <v>348.3043291691101</v>
+        <v>389.6204369257978</v>
       </c>
       <c r="G13" t="n">
-        <v>971.5298031763974</v>
+        <v>1040.876859605055</v>
       </c>
       <c r="H13" t="n">
-        <v>5145.32275629334</v>
+        <v>5119.305215033213</v>
       </c>
       <c r="I13" t="n">
-        <v>21666.25232366338</v>
+        <v>21458.54452577989</v>
       </c>
       <c r="J13" t="n">
-        <v>45241.12625704035</v>
+        <v>45463.29572923431</v>
       </c>
       <c r="K13" t="n">
-        <v>68417.79296713643</v>
+        <v>67437.73694936236</v>
       </c>
       <c r="L13" t="n">
-        <v>112658.3617761035</v>
+        <v>110978.370606496</v>
       </c>
       <c r="M13" t="n">
-        <v>242424.6216362597</v>
+        <v>223139.2014001834</v>
       </c>
       <c r="N13" t="n">
-        <v>459708.3834819635</v>
+        <v>406937.2898310228</v>
       </c>
       <c r="O13" t="s">
         <v>37</v>
       </c>
       <c r="P13" t="n">
-        <v>945.1821577577185</v>
+        <v>847.2388740255942</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.01415470230398636</v>
+        <v>0.01379329447799939</v>
       </c>
       <c r="R13" t="s"/>
       <c r="S13" t="s">
@@ -1320,52 +1320,52 @@
         <v>38</v>
       </c>
       <c r="B14" t="n">
-        <v>225.6575134636092</v>
+        <v>242.5139218281163</v>
       </c>
       <c r="C14" t="n">
-        <v>416.2413695233791</v>
+        <v>442.7104574874</v>
       </c>
       <c r="D14" t="n">
-        <v>838.4710820243786</v>
+        <v>877.6016863714352</v>
       </c>
       <c r="E14" t="n">
-        <v>1351.679701638263</v>
+        <v>1409.9812976542</v>
       </c>
       <c r="F14" t="n">
-        <v>1968.12705430113</v>
+        <v>2098.880186408528</v>
       </c>
       <c r="G14" t="n">
-        <v>3813.440453635915</v>
+        <v>4003.743022825235</v>
       </c>
       <c r="H14" t="n">
-        <v>12145.89852677416</v>
+        <v>11997.44703762381</v>
       </c>
       <c r="I14" t="n">
-        <v>43188.64021216847</v>
+        <v>42340.87620811316</v>
       </c>
       <c r="J14" t="n">
-        <v>106565.2417764303</v>
+        <v>103425.8569594839</v>
       </c>
       <c r="K14" t="n">
-        <v>191279.2143253468</v>
+        <v>185874.3606667948</v>
       </c>
       <c r="L14" t="n">
-        <v>411336.7169863478</v>
+        <v>391154.3001312229</v>
       </c>
       <c r="M14" t="n">
-        <v>1312065.430702387</v>
+        <v>1229864.895552056</v>
       </c>
       <c r="N14" t="n">
-        <v>3697835.984460949</v>
+        <v>3351690.146720767</v>
       </c>
       <c r="O14" t="s">
         <v>38</v>
       </c>
       <c r="P14" t="n">
-        <v>449752.8376737849</v>
+        <v>364884.3950483791</v>
       </c>
       <c r="Q14" t="n">
-        <v>3624.005286656417</v>
+        <v>3558.495710421128</v>
       </c>
       <c r="R14" t="s"/>
       <c r="S14" t="s">
@@ -1405,52 +1405,52 @@
         <v>39</v>
       </c>
       <c r="B15" t="n">
-        <v>292.6778111140152</v>
+        <v>311.2652658225011</v>
       </c>
       <c r="C15" t="n">
-        <v>530.7464079724365</v>
+        <v>546.4277184056085</v>
       </c>
       <c r="D15" t="n">
-        <v>1018.38916737331</v>
+        <v>1080.210352850189</v>
       </c>
       <c r="E15" t="n">
-        <v>1655.656020162027</v>
+        <v>1650.193297963018</v>
       </c>
       <c r="F15" t="n">
-        <v>2372.269142189435</v>
+        <v>2381.712108074881</v>
       </c>
       <c r="G15" t="n">
-        <v>4264.242409280171</v>
+        <v>4435.010143342875</v>
       </c>
       <c r="H15" t="n">
-        <v>12956.7036382359</v>
+        <v>12935.91721388257</v>
       </c>
       <c r="I15" t="n">
-        <v>44897.32752652139</v>
+        <v>45416.42741029997</v>
       </c>
       <c r="J15" t="n">
-        <v>112509.4855250122</v>
+        <v>112304.9867281014</v>
       </c>
       <c r="K15" t="n">
-        <v>211011.8154182836</v>
+        <v>203531.5091311389</v>
       </c>
       <c r="L15" t="n">
-        <v>463401.6663801415</v>
+        <v>444278.0369198282</v>
       </c>
       <c r="M15" t="n">
-        <v>1482621.51905109</v>
+        <v>1468811.455780063</v>
       </c>
       <c r="N15" t="n">
-        <v>4190571.955619165</v>
+        <v>3977200.433331154</v>
       </c>
       <c r="O15" t="s">
         <v>39</v>
       </c>
       <c r="P15" t="n">
-        <v>561245.8378845219</v>
+        <v>447121.2054627783</v>
       </c>
       <c r="Q15" t="n">
-        <v>4961.433466698427</v>
+        <v>4446.481593383473</v>
       </c>
       <c r="R15" t="s"/>
       <c r="S15" t="s">

</xml_diff>

<commit_message>
Functionnal Log Empirical (Validation comming soon)
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -1065,52 +1065,52 @@
         <v>33</v>
       </c>
       <c r="B11" t="n">
-        <v>2.523952683481694</v>
+        <v>2.456562955918035</v>
       </c>
       <c r="C11" t="n">
-        <v>2.245557781762061</v>
+        <v>2.19437524839901</v>
       </c>
       <c r="D11" t="n">
-        <v>1.965292524346421</v>
+        <v>1.929309426301781</v>
       </c>
       <c r="E11" t="n">
-        <v>1.798699734995178</v>
+        <v>1.771151378621231</v>
       </c>
       <c r="F11" t="n">
-        <v>1.678489209171317</v>
+        <v>1.656714689475387</v>
       </c>
       <c r="G11" t="n">
-        <v>1.50549253076452</v>
+        <v>1.491495282503209</v>
       </c>
       <c r="H11" t="n">
-        <v>1.29005654150989</v>
+        <v>1.284310394533257</v>
       </c>
       <c r="I11" t="n">
-        <v>1.228425208407695</v>
+        <v>1.221512320766259</v>
       </c>
       <c r="J11" t="n">
-        <v>1.296715213156989</v>
+        <v>1.284309112159226</v>
       </c>
       <c r="K11" t="n">
-        <v>1.366467934507143</v>
+        <v>1.349883082319397</v>
       </c>
       <c r="L11" t="n">
-        <v>1.474669289784171</v>
+        <v>1.45206771735443</v>
       </c>
       <c r="M11" t="n">
-        <v>1.668651422839158</v>
+        <v>1.635319667627088</v>
       </c>
       <c r="N11" t="n">
-        <v>1.866958557192161</v>
+        <v>1.822218474612457</v>
       </c>
       <c r="O11" t="s">
         <v>33</v>
       </c>
       <c r="P11" t="n">
-        <v>12.43528614073925</v>
+        <v>12.30642387490133</v>
       </c>
       <c r="Q11" t="n">
-        <v>109.1068896340253</v>
+        <v>108.5025798185205</v>
       </c>
       <c r="R11" t="s"/>
       <c r="S11" t="s">
@@ -1150,52 +1150,52 @@
         <v>34</v>
       </c>
       <c r="B12" t="n">
-        <v>8.636587370982896</v>
+        <v>8.017715864205524</v>
       </c>
       <c r="C12" t="n">
-        <v>24.51602330310273</v>
+        <v>22.79975815571148</v>
       </c>
       <c r="D12" t="n">
-        <v>82.10444858633001</v>
+        <v>74.91494376403058</v>
       </c>
       <c r="E12" t="n">
-        <v>182.3540481148718</v>
+        <v>169.8751889981022</v>
       </c>
       <c r="F12" t="n">
-        <v>337.667636511364</v>
+        <v>323.5070013396253</v>
       </c>
       <c r="G12" t="n">
-        <v>937.7923046339511</v>
+        <v>909.60275055444</v>
       </c>
       <c r="H12" t="n">
-        <v>4783.045713271225</v>
+        <v>4786.807581718066</v>
       </c>
       <c r="I12" t="n">
-        <v>20657.72492187663</v>
+        <v>20950.28860513512</v>
       </c>
       <c r="J12" t="n">
-        <v>41559.42746431254</v>
+        <v>42999.52299722662</v>
       </c>
       <c r="K12" t="n">
-        <v>61482.02086622499</v>
+        <v>64105.41848637789</v>
       </c>
       <c r="L12" t="n">
-        <v>99227.79640890517</v>
+        <v>104405.471529214</v>
       </c>
       <c r="M12" t="n">
-        <v>194008.5614032715</v>
+        <v>209799.0981969993</v>
       </c>
       <c r="N12" t="n">
-        <v>354829.3493756181</v>
+        <v>396908.5412955568</v>
       </c>
       <c r="O12" t="s">
         <v>34</v>
       </c>
       <c r="P12" t="n">
-        <v>763.3388887773664</v>
+        <v>755.0326324959477</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.01150516414986073</v>
+        <v>0.0123243458632216</v>
       </c>
       <c r="R12" t="s"/>
       <c r="S12" t="s">
@@ -1235,52 +1235,52 @@
         <v>37</v>
       </c>
       <c r="B13" t="n">
-        <v>12.03155630896678</v>
+        <v>10.92948232981785</v>
       </c>
       <c r="C13" t="n">
-        <v>31.38551582130729</v>
+        <v>29.79744920846311</v>
       </c>
       <c r="D13" t="n">
-        <v>98.2360995451056</v>
+        <v>96.40877207134318</v>
       </c>
       <c r="E13" t="n">
-        <v>210.7505610033742</v>
+        <v>206.6240388255761</v>
       </c>
       <c r="F13" t="n">
-        <v>389.6204369257978</v>
+        <v>381.1608749802875</v>
       </c>
       <c r="G13" t="n">
-        <v>1040.876859605055</v>
+        <v>1054.928922715712</v>
       </c>
       <c r="H13" t="n">
-        <v>5119.305215033213</v>
+        <v>5126.185448057211</v>
       </c>
       <c r="I13" t="n">
-        <v>21458.54452577989</v>
+        <v>22549.13486675487</v>
       </c>
       <c r="J13" t="n">
-        <v>45463.29572923431</v>
+        <v>47173.38963892015</v>
       </c>
       <c r="K13" t="n">
-        <v>67437.73694936236</v>
+        <v>70767.65919831787</v>
       </c>
       <c r="L13" t="n">
-        <v>110978.370606496</v>
+        <v>117352.8911064405</v>
       </c>
       <c r="M13" t="n">
-        <v>223139.2014001834</v>
+        <v>244032.1418783148</v>
       </c>
       <c r="N13" t="n">
-        <v>406937.2898310228</v>
+        <v>470579.0374273685</v>
       </c>
       <c r="O13" t="s">
         <v>37</v>
       </c>
       <c r="P13" t="n">
-        <v>847.2388740255942</v>
+        <v>834.3759748810188</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.01379329447799939</v>
+        <v>0.01364721961043449</v>
       </c>
       <c r="R13" t="s"/>
       <c r="S13" t="s">
@@ -1320,52 +1320,52 @@
         <v>38</v>
       </c>
       <c r="B14" t="n">
-        <v>242.5139218281163</v>
+        <v>210.2416781845095</v>
       </c>
       <c r="C14" t="n">
-        <v>442.7104574874</v>
+        <v>392.9484143461237</v>
       </c>
       <c r="D14" t="n">
-        <v>877.6016863714352</v>
+        <v>813.5260624818053</v>
       </c>
       <c r="E14" t="n">
-        <v>1409.9812976542</v>
+        <v>1350.583747859673</v>
       </c>
       <c r="F14" t="n">
-        <v>2098.880186408528</v>
+        <v>2004.236308563269</v>
       </c>
       <c r="G14" t="n">
-        <v>4003.743022825235</v>
+        <v>3885.597291372204</v>
       </c>
       <c r="H14" t="n">
-        <v>11997.44703762381</v>
+        <v>11725.33977588181</v>
       </c>
       <c r="I14" t="n">
-        <v>42340.87620811316</v>
+        <v>43842.84805320212</v>
       </c>
       <c r="J14" t="n">
-        <v>103425.8569594839</v>
+        <v>106306.5703389645</v>
       </c>
       <c r="K14" t="n">
-        <v>185874.3606667948</v>
+        <v>187776.4635616026</v>
       </c>
       <c r="L14" t="n">
-        <v>391154.3001312229</v>
+        <v>399999.8604810955</v>
       </c>
       <c r="M14" t="n">
-        <v>1229864.895552056</v>
+        <v>1229583.098692825</v>
       </c>
       <c r="N14" t="n">
-        <v>3351690.146720767</v>
+        <v>3352198.553081083</v>
       </c>
       <c r="O14" t="s">
         <v>38</v>
       </c>
       <c r="P14" t="n">
-        <v>364884.3950483791</v>
+        <v>357225.9762336689</v>
       </c>
       <c r="Q14" t="n">
-        <v>3558.495710421128</v>
+        <v>3620.895275051425</v>
       </c>
       <c r="R14" t="s"/>
       <c r="S14" t="s">
@@ -1405,52 +1405,52 @@
         <v>39</v>
       </c>
       <c r="B15" t="n">
-        <v>311.2652658225011</v>
+        <v>263.4849411850086</v>
       </c>
       <c r="C15" t="n">
-        <v>546.4277184056085</v>
+        <v>486.498976784299</v>
       </c>
       <c r="D15" t="n">
-        <v>1080.210352850189</v>
+        <v>964.3505987289286</v>
       </c>
       <c r="E15" t="n">
-        <v>1650.193297963018</v>
+        <v>1569.598203221606</v>
       </c>
       <c r="F15" t="n">
-        <v>2381.712108074881</v>
+        <v>2264.506397347969</v>
       </c>
       <c r="G15" t="n">
-        <v>4435.010143342875</v>
+        <v>4370.415073081558</v>
       </c>
       <c r="H15" t="n">
-        <v>12935.91721388257</v>
+        <v>12951.03975876778</v>
       </c>
       <c r="I15" t="n">
-        <v>45416.42741029997</v>
+        <v>46449.75731883464</v>
       </c>
       <c r="J15" t="n">
-        <v>112304.9867281014</v>
+        <v>115996.5245748017</v>
       </c>
       <c r="K15" t="n">
-        <v>203531.5091311389</v>
+        <v>212480.2347236348</v>
       </c>
       <c r="L15" t="n">
-        <v>444278.0369198282</v>
+        <v>455533.7624090513</v>
       </c>
       <c r="M15" t="n">
-        <v>1468811.455780063</v>
+        <v>1427513.066045994</v>
       </c>
       <c r="N15" t="n">
-        <v>3977200.433331154</v>
+        <v>3963156.854017044</v>
       </c>
       <c r="O15" t="s">
         <v>39</v>
       </c>
       <c r="P15" t="n">
-        <v>447121.2054627783</v>
+        <v>428796.1457255174</v>
       </c>
       <c r="Q15" t="n">
-        <v>4446.481593383473</v>
+        <v>4341.762131528685</v>
       </c>
       <c r="R15" t="s"/>
       <c r="S15" t="s">

</xml_diff>